<commit_message>
Added sample data files
</commit_message>
<xml_diff>
--- a/Documentation/About/ForumID_Details.xlsx
+++ b/Documentation/About/ForumID_Details.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aruna\Documents\ACMS-IID\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aruna\Documents\ACMS-IID\documentation\about\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="505">
   <si>
     <t>Performance Insights</t>
   </si>
@@ -1530,18 +1530,6 @@
   </si>
   <si>
     <t>Not scraped because the forum is in another language</t>
-  </si>
-  <si>
-    <t>Work Assigned To</t>
-  </si>
-  <si>
-    <t>Geetha</t>
-  </si>
-  <si>
-    <t>Kavya</t>
-  </si>
-  <si>
-    <t>Aruna</t>
   </si>
   <si>
     <t>Forums are redundant</t>
@@ -1557,14 +1545,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1582,14 +1563,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1617,7 +1590,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1634,68 +1607,13 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top/>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1708,72 +1626,42 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="40% - Accent1" xfId="3" builtinId="31"/>
-    <cellStyle name="40% - Accent2" xfId="4" builtinId="35"/>
-    <cellStyle name="40% - Accent6" xfId="5" builtinId="51"/>
+  <cellStyles count="3">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2054,10 +1942,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D267"/>
+  <dimension ref="A1:C266"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="D2" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2065,11 +1953,10 @@
     <col min="1" max="1" width="61.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.44140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="38.77734375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="2"/>
+    <col min="4" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" s="5" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>499</v>
       </c>
@@ -2077,629 +1964,554 @@
         <v>500</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>508</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="7"/>
-    </row>
-    <row r="4" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="7"/>
-    </row>
-    <row r="5" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="7"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="7"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="7"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="7"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="7"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="7"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="7"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="7"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="7"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="7"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="7"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="7"/>
-    </row>
-    <row r="17" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:2" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="7"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="7"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="7"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="7"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="7"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D22" s="7"/>
-    </row>
-    <row r="23" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:2" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="7"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D24" s="7"/>
-    </row>
-    <row r="25" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:2" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D25" s="7"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="7"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D27" s="7"/>
-    </row>
-    <row r="28" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:2" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D28" s="7"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D29" s="7"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D30" s="7"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D31" s="7"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D32" s="7"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D33" s="7"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D34" s="7"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D35" s="7"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D36" s="7"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D37" s="7"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D38" s="7"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D39" s="7"/>
-    </row>
-    <row r="40" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:2" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>76</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D40" s="7"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D41" s="7"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D42" s="7"/>
-    </row>
-    <row r="43" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:2" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>82</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D43" s="7"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D44" s="7"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D45" s="7"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>88</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D46" s="7"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D47" s="7"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D48" s="7"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>94</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D49" s="7"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>96</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D50" s="7"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>98</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D51" s="7"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>100</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D52" s="7"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>102</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D53" s="7"/>
-    </row>
-    <row r="54" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="54" spans="1:2" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>104</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="D54" s="7"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>106</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D55" s="7"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>108</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D56" s="7"/>
-    </row>
-    <row r="57" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="57" spans="1:2" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>110</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D57" s="7"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D58" s="7"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>114</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D59" s="7"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>116</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D60" s="7"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>118</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D61" s="7"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>120</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D62" s="7"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>122</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="D63" s="7"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>124</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="D64" s="7"/>
-    </row>
-    <row r="65" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="65" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
         <v>126</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="D65" s="7"/>
-    </row>
-    <row r="66" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>128</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="D66" s="8"/>
-    </row>
-    <row r="67" spans="1:4" s="1" customFormat="1" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="67" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
         <v>130</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="D67" s="9" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>132</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D68" s="10"/>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>134</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="D69" s="10"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>136</v>
       </c>
@@ -2709,9 +2521,8 @@
       <c r="C70" s="2">
         <v>18</v>
       </c>
-      <c r="D70" s="10"/>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>138</v>
       </c>
@@ -2721,9 +2532,8 @@
       <c r="C71" s="2">
         <v>74</v>
       </c>
-      <c r="D71" s="10"/>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>140</v>
       </c>
@@ -2733,9 +2543,8 @@
       <c r="C72" s="2">
         <v>12</v>
       </c>
-      <c r="D72" s="10"/>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>142</v>
       </c>
@@ -2745,841 +2554,745 @@
       <c r="C73" s="2">
         <v>14</v>
       </c>
-      <c r="D73" s="10"/>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>144</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C74" s="17" t="s">
-        <v>507</v>
-      </c>
-      <c r="D74" s="10"/>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C74" s="9" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>146</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C75" s="17"/>
-      <c r="D75" s="10"/>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C75" s="9"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>148</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C76" s="17"/>
-      <c r="D76" s="10"/>
-    </row>
-    <row r="77" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C76" s="9"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>150</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C77" s="17"/>
-      <c r="D77" s="11"/>
-    </row>
-    <row r="78" spans="1:4" s="1" customFormat="1" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="C77" s="9"/>
+    </row>
+    <row r="78" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
         <v>152</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="D78" s="14" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>154</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="D79" s="15"/>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>156</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="D80" s="15"/>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>158</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="D81" s="15"/>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>160</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="D82" s="15"/>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>162</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="D83" s="15"/>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>164</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="D84" s="15"/>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>166</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="D85" s="15"/>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>168</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="D86" s="15"/>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>170</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="D87" s="15"/>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>172</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="D88" s="15"/>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>174</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="D89" s="15"/>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>176</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="D90" s="15"/>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>178</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="D91" s="15"/>
-    </row>
-    <row r="92" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="92" spans="1:2" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
         <v>180</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="D92" s="15"/>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>182</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="D93" s="15"/>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>184</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="D94" s="15"/>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>186</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="D95" s="15"/>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>188</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="D96" s="15"/>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>190</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="D97" s="15"/>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>192</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="D98" s="15"/>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>194</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="D99" s="15"/>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>196</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="D100" s="15"/>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>198</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="D101" s="15"/>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>200</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="D102" s="15"/>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>202</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="D103" s="15"/>
-    </row>
-    <row r="104" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="104" spans="1:2" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
         <v>204</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="D104" s="15"/>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>206</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="D105" s="15"/>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>208</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="D106" s="15"/>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>210</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="D107" s="15"/>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>212</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="D108" s="15"/>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>214</v>
       </c>
       <c r="B109" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="D109" s="15"/>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>216</v>
       </c>
       <c r="B110" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="D110" s="15"/>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>218</v>
       </c>
       <c r="B111" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="D111" s="15"/>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>220</v>
       </c>
       <c r="B112" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="D112" s="15"/>
-    </row>
-    <row r="113" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="113" spans="1:2" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A113" s="3" t="s">
         <v>222</v>
       </c>
       <c r="B113" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="D113" s="15"/>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>224</v>
       </c>
       <c r="B114" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="D114" s="15"/>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>226</v>
       </c>
       <c r="B115" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="D115" s="15"/>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>228</v>
       </c>
       <c r="B116" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="D116" s="15"/>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>230</v>
       </c>
       <c r="B117" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="D117" s="15"/>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>232</v>
       </c>
       <c r="B118" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="D118" s="15"/>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>234</v>
       </c>
       <c r="B119" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="D119" s="15"/>
-    </row>
-    <row r="120" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="120" spans="1:2" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A120" s="3" t="s">
         <v>236</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="D120" s="15"/>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>238</v>
       </c>
       <c r="B121" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="D121" s="15"/>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>240</v>
       </c>
       <c r="B122" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="D122" s="15"/>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>242</v>
       </c>
       <c r="B123" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="D123" s="15"/>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>244</v>
       </c>
       <c r="B124" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="D124" s="15"/>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>246</v>
       </c>
       <c r="B125" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="D125" s="15"/>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>248</v>
       </c>
       <c r="B126" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="D126" s="15"/>
-    </row>
-    <row r="127" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="127" spans="1:2" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A127" s="3" t="s">
         <v>250</v>
       </c>
       <c r="B127" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="D127" s="15"/>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>252</v>
       </c>
       <c r="B128" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="D128" s="15"/>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>254</v>
       </c>
       <c r="B129" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="D129" s="15"/>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>256</v>
       </c>
       <c r="B130" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="D130" s="15"/>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>258</v>
       </c>
       <c r="B131" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="D131" s="15"/>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>260</v>
       </c>
       <c r="B132" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="D132" s="15"/>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>262</v>
       </c>
       <c r="B133" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="D133" s="15"/>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>264</v>
       </c>
       <c r="B134" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="D134" s="15"/>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>266</v>
       </c>
       <c r="B135" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="D135" s="15"/>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>268</v>
       </c>
       <c r="B136" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="D136" s="15"/>
-    </row>
-    <row r="137" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="137" spans="1:2" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A137" s="3" t="s">
         <v>270</v>
       </c>
       <c r="B137" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="D137" s="15"/>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>272</v>
       </c>
       <c r="B138" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="D138" s="15"/>
-    </row>
-    <row r="139" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="139" spans="1:2" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A139" s="3" t="s">
         <v>274</v>
       </c>
       <c r="B139" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="D139" s="10" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
         <v>276</v>
       </c>
       <c r="B140" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="D140" s="10"/>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
         <v>278</v>
       </c>
       <c r="B141" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="D141" s="10"/>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
         <v>280</v>
       </c>
       <c r="B142" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="D142" s="10"/>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
         <v>282</v>
       </c>
       <c r="B143" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="D143" s="10"/>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
         <v>284</v>
       </c>
       <c r="B144" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="D144" s="10"/>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
         <v>286</v>
       </c>
       <c r="B145" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="D145" s="10"/>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
         <v>288</v>
       </c>
       <c r="B146" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="D146" s="10"/>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
         <v>290</v>
       </c>
       <c r="B147" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="D147" s="10"/>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
         <v>292</v>
       </c>
       <c r="B148" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="D148" s="10"/>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
         <v>294</v>
       </c>
       <c r="B149" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="D149" s="10"/>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
         <v>296</v>
       </c>
       <c r="B150" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="D150" s="10"/>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
         <v>298</v>
       </c>
       <c r="B151" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="D151" s="10"/>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
         <v>300</v>
       </c>
       <c r="B152" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="D152" s="10"/>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
         <v>302</v>
       </c>
       <c r="B153" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="C153" s="16" t="s">
-        <v>507</v>
-      </c>
-      <c r="D153" s="10"/>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C153" s="6" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
         <v>304</v>
       </c>
       <c r="B154" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="D154" s="10"/>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" s="2" t="s">
         <v>306</v>
       </c>
       <c r="B155" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="D155" s="10"/>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
         <v>308</v>
       </c>
       <c r="B156" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="D156" s="10"/>
-    </row>
-    <row r="157" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="157" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A157" s="3" t="s">
         <v>310</v>
       </c>
       <c r="B157" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="D157" s="10"/>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158" s="2" t="s">
         <v>312</v>
       </c>
       <c r="B158" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="D158" s="10"/>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" s="2" t="s">
         <v>314</v>
       </c>
       <c r="B159" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="D159" s="10"/>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" s="2" t="s">
         <v>316</v>
       </c>
       <c r="B160" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="D160" s="10"/>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" s="2" t="s">
         <v>318</v>
       </c>
       <c r="B161" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="D161" s="10"/>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" s="2" t="s">
         <v>320</v>
       </c>
       <c r="B162" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="D162" s="10"/>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" s="2" t="s">
         <v>322</v>
       </c>
       <c r="B163" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="D163" s="10"/>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" s="2" t="s">
         <v>324</v>
       </c>
       <c r="B164" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="D164" s="10"/>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" s="2" t="s">
         <v>326</v>
       </c>
@@ -3587,142 +3300,127 @@
         <v>327</v>
       </c>
       <c r="C165" s="4" t="s">
-        <v>507</v>
-      </c>
-      <c r="D165" s="10"/>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" s="2" t="s">
         <v>328</v>
       </c>
       <c r="B166" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="D166" s="10"/>
-    </row>
-    <row r="167" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="167" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A167" s="3" t="s">
         <v>330</v>
       </c>
       <c r="B167" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="D167" s="10"/>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" s="2" t="s">
         <v>332</v>
       </c>
       <c r="B168" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="D168" s="10"/>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" s="2" t="s">
         <v>334</v>
       </c>
       <c r="B169" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="D169" s="10"/>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" s="2" t="s">
         <v>336</v>
       </c>
       <c r="B170" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="D170" s="10"/>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" s="2" t="s">
         <v>338</v>
       </c>
       <c r="B171" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="D171" s="10"/>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" s="2" t="s">
         <v>340</v>
       </c>
       <c r="B172" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="D172" s="10"/>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" s="2" t="s">
         <v>342</v>
       </c>
       <c r="B173" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="D173" s="10"/>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" s="2" t="s">
         <v>344</v>
       </c>
       <c r="B174" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="D174" s="10"/>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" s="2" t="s">
         <v>346</v>
       </c>
       <c r="B175" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="D175" s="10"/>
-    </row>
-    <row r="176" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="176" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A176" s="3" t="s">
         <v>348</v>
       </c>
       <c r="B176" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="C176" s="13" t="s">
-        <v>507</v>
-      </c>
-      <c r="D176" s="10"/>
-    </row>
-    <row r="177" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C176" s="8" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A177" s="3" t="s">
         <v>350</v>
       </c>
       <c r="B177" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="C177" s="13"/>
-      <c r="D177" s="10"/>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C177" s="8"/>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178" s="2" t="s">
         <v>350</v>
       </c>
       <c r="B178" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="C178" s="13"/>
-      <c r="D178" s="10"/>
-    </row>
-    <row r="179" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C178" s="8"/>
+    </row>
+    <row r="179" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A179" s="3" t="s">
         <v>353</v>
       </c>
       <c r="B179" s="3" t="s">
         <v>354</v>
       </c>
-      <c r="D179" s="10"/>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180" s="2" t="s">
         <v>355</v>
       </c>
@@ -3730,856 +3428,764 @@
         <v>356</v>
       </c>
       <c r="C180" s="4" t="s">
-        <v>507</v>
-      </c>
-      <c r="D180" s="10"/>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" s="2" t="s">
         <v>357</v>
       </c>
       <c r="B181" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="D181" s="10"/>
-    </row>
-    <row r="182" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="182" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A182" s="3" t="s">
         <v>359</v>
       </c>
       <c r="B182" s="3" t="s">
         <v>360</v>
       </c>
-      <c r="D182" s="10"/>
-    </row>
-    <row r="183" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="183" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A183" s="3" t="s">
         <v>361</v>
       </c>
       <c r="B183" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="D183" s="10"/>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184" s="2" t="s">
         <v>361</v>
       </c>
       <c r="B184" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="D184" s="10"/>
-    </row>
-    <row r="185" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="185" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A185" s="3" t="s">
         <v>364</v>
       </c>
       <c r="B185" s="3" t="s">
         <v>365</v>
       </c>
-      <c r="D185" s="10"/>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A186" s="2" t="s">
         <v>364</v>
       </c>
       <c r="B186" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="D186" s="10"/>
-    </row>
-    <row r="187" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="187" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A187" s="3" t="s">
         <v>367</v>
       </c>
       <c r="B187" s="3" t="s">
         <v>368</v>
       </c>
-      <c r="D187" s="10"/>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A188" s="2" t="s">
         <v>369</v>
       </c>
       <c r="B188" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="D188" s="10"/>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A189" s="2" t="s">
         <v>371</v>
       </c>
       <c r="B189" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="D189" s="10"/>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A190" s="2" t="s">
         <v>373</v>
       </c>
       <c r="B190" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="D190" s="10"/>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A191" s="2" t="s">
         <v>375</v>
       </c>
       <c r="B191" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="D191" s="10"/>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A192" s="2" t="s">
         <v>377</v>
       </c>
       <c r="B192" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="D192" s="10"/>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A193" s="2" t="s">
         <v>379</v>
       </c>
       <c r="B193" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="D193" s="10"/>
-    </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194" s="2" t="s">
         <v>381</v>
       </c>
       <c r="B194" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="D194" s="10"/>
-    </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A195" s="2" t="s">
         <v>383</v>
       </c>
       <c r="B195" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="D195" s="10"/>
-    </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A196" s="2" t="s">
         <v>385</v>
       </c>
       <c r="B196" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="D196" s="10"/>
-    </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A197" s="2" t="s">
         <v>387</v>
       </c>
       <c r="B197" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="D197" s="10"/>
-    </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A198" s="2" t="s">
         <v>389</v>
       </c>
       <c r="B198" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="D198" s="10"/>
-    </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A199" s="2" t="s">
         <v>391</v>
       </c>
       <c r="B199" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="D199" s="10"/>
-    </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A200" s="2" t="s">
         <v>393</v>
       </c>
       <c r="B200" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="D200" s="10"/>
-    </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A201" s="2" t="s">
         <v>395</v>
       </c>
       <c r="B201" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="D201" s="10"/>
-    </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A202" s="2" t="s">
         <v>397</v>
       </c>
       <c r="B202" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="D202" s="10"/>
-    </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A203" s="2" t="s">
         <v>399</v>
       </c>
       <c r="B203" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="D203" s="10"/>
-    </row>
-    <row r="204" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="204" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A204" s="3" t="s">
         <v>401</v>
       </c>
       <c r="B204" s="3" t="s">
         <v>402</v>
       </c>
-      <c r="D204" s="10"/>
-    </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A205" s="2" t="s">
         <v>110</v>
       </c>
       <c r="B205" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="D205" s="10"/>
-    </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A206" s="2" t="s">
         <v>404</v>
       </c>
       <c r="B206" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="D206" s="10"/>
-    </row>
-    <row r="207" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="207" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A207" s="3" t="s">
         <v>406</v>
       </c>
       <c r="B207" s="3" t="s">
         <v>407</v>
       </c>
-      <c r="C207" s="12" t="s">
+      <c r="C207" s="7" t="s">
         <v>501</v>
       </c>
-      <c r="D207" s="10"/>
-    </row>
-    <row r="208" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="208" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A208" s="3" t="s">
         <v>408</v>
       </c>
       <c r="B208" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="C208" s="12"/>
-      <c r="D208" s="10"/>
-    </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C208" s="7"/>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A209" s="2" t="s">
         <v>410</v>
       </c>
       <c r="B209" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="C209" s="12"/>
-      <c r="D209" s="10"/>
-    </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C209" s="7"/>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A210" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B210" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="C210" s="12"/>
-      <c r="D210" s="10"/>
-    </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C210" s="7"/>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A211" s="2" t="s">
         <v>413</v>
       </c>
       <c r="B211" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="C211" s="12"/>
-      <c r="D211" s="10"/>
-    </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C211" s="7"/>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A212" s="2" t="s">
         <v>258</v>
       </c>
       <c r="B212" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="C212" s="12"/>
-      <c r="D212" s="10"/>
-    </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C212" s="7"/>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A213" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B213" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="C213" s="12"/>
-      <c r="D213" s="10"/>
-    </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C213" s="7"/>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A214" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B214" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="C214" s="12"/>
-      <c r="D214" s="10"/>
-    </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C214" s="7"/>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A215" s="2" t="s">
         <v>256</v>
       </c>
       <c r="B215" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="C215" s="12"/>
-      <c r="D215" s="10"/>
-    </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C215" s="7"/>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A216" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B216" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="C216" s="12"/>
-      <c r="D216" s="10"/>
-    </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C216" s="7"/>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A217" s="2" t="s">
         <v>338</v>
       </c>
       <c r="B217" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="C217" s="12"/>
-      <c r="D217" s="10"/>
-    </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C217" s="7"/>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A218" s="2" t="s">
         <v>332</v>
       </c>
       <c r="B218" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="C218" s="12"/>
-      <c r="D218" s="10"/>
-    </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C218" s="7"/>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A219" s="2" t="s">
         <v>422</v>
       </c>
       <c r="B219" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="C219" s="12"/>
-      <c r="D219" s="10"/>
-    </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C219" s="7"/>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A220" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B220" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="C220" s="12"/>
-      <c r="D220" s="10"/>
-    </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C220" s="7"/>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A221" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B221" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="C221" s="12"/>
-      <c r="D221" s="10"/>
-    </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C221" s="7"/>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A222" s="2" t="s">
         <v>334</v>
       </c>
       <c r="B222" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="C222" s="12"/>
-      <c r="D222" s="10"/>
-    </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C222" s="7"/>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A223" s="2" t="s">
         <v>316</v>
       </c>
       <c r="B223" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="C223" s="12"/>
-      <c r="D223" s="10"/>
-    </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C223" s="7"/>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A224" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B224" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="C224" s="12"/>
-      <c r="D224" s="10"/>
-    </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C224" s="7"/>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A225" s="2" t="s">
         <v>276</v>
       </c>
       <c r="B225" s="2" t="s">
         <v>429</v>
       </c>
-      <c r="C225" s="12"/>
-      <c r="D225" s="10"/>
-    </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C225" s="7"/>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A226" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B226" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="C226" s="12"/>
-      <c r="D226" s="10"/>
-    </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C226" s="7"/>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A227" s="2" t="s">
         <v>254</v>
       </c>
       <c r="B227" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="C227" s="12"/>
-      <c r="D227" s="10"/>
-    </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C227" s="7"/>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A228" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B228" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="C228" s="12"/>
-      <c r="D228" s="10"/>
-    </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C228" s="7"/>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A229" s="2" t="s">
         <v>182</v>
       </c>
       <c r="B229" s="2" t="s">
         <v>433</v>
       </c>
-      <c r="C229" s="12"/>
-      <c r="D229" s="10"/>
-    </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C229" s="7"/>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A230" s="2" t="s">
         <v>94</v>
       </c>
       <c r="B230" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="C230" s="12"/>
-      <c r="D230" s="10"/>
-    </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C230" s="7"/>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A231" s="2" t="s">
         <v>318</v>
       </c>
       <c r="B231" s="2" t="s">
         <v>435</v>
       </c>
-      <c r="C231" s="12"/>
-      <c r="D231" s="10"/>
-    </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C231" s="7"/>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A232" s="2" t="s">
         <v>340</v>
       </c>
       <c r="B232" s="2" t="s">
         <v>436</v>
       </c>
-      <c r="C232" s="12"/>
-      <c r="D232" s="10"/>
-    </row>
-    <row r="233" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C232" s="7"/>
+    </row>
+    <row r="233" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A233" s="3" t="s">
         <v>437</v>
       </c>
       <c r="B233" s="3" t="s">
         <v>438</v>
       </c>
-      <c r="C233" s="12"/>
-      <c r="D233" s="10"/>
-    </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C233" s="7"/>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A234" s="2" t="s">
         <v>439</v>
       </c>
       <c r="B234" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="C234" s="12"/>
-      <c r="D234" s="10"/>
-    </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C234" s="7"/>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A235" s="2" t="s">
         <v>373</v>
       </c>
       <c r="B235" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="C235" s="12"/>
-      <c r="D235" s="10"/>
-    </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C235" s="7"/>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A236" s="2" t="s">
         <v>442</v>
       </c>
       <c r="B236" s="2" t="s">
         <v>443</v>
       </c>
-      <c r="C236" s="12"/>
-      <c r="D236" s="10"/>
-    </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C236" s="7"/>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A237" s="2" t="s">
         <v>379</v>
       </c>
       <c r="B237" s="2" t="s">
         <v>444</v>
       </c>
-      <c r="C237" s="12"/>
-      <c r="D237" s="10"/>
-    </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C237" s="7"/>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A238" s="2" t="s">
         <v>445</v>
       </c>
       <c r="B238" s="2" t="s">
         <v>446</v>
       </c>
-      <c r="C238" s="12"/>
-      <c r="D238" s="10"/>
-    </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C238" s="7"/>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A239" s="2" t="s">
         <v>447</v>
       </c>
       <c r="B239" s="2" t="s">
         <v>448</v>
       </c>
-      <c r="C239" s="12"/>
-      <c r="D239" s="10"/>
-    </row>
-    <row r="240" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C239" s="7"/>
+    </row>
+    <row r="240" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A240" s="3" t="s">
         <v>449</v>
       </c>
       <c r="B240" s="3" t="s">
         <v>450</v>
       </c>
-      <c r="C240" s="12"/>
-      <c r="D240" s="10"/>
-    </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C240" s="7"/>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A241" s="2" t="s">
         <v>451</v>
       </c>
       <c r="B241" s="2" t="s">
         <v>452</v>
       </c>
-      <c r="C241" s="12"/>
-      <c r="D241" s="10"/>
-    </row>
-    <row r="242" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C241" s="7"/>
+    </row>
+    <row r="242" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A242" s="3" t="s">
         <v>453</v>
       </c>
       <c r="B242" s="3" t="s">
         <v>454</v>
       </c>
-      <c r="C242" s="12"/>
-      <c r="D242" s="10"/>
-    </row>
-    <row r="243" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C242" s="7"/>
+    </row>
+    <row r="243" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A243" s="3" t="s">
         <v>455</v>
       </c>
       <c r="B243" s="3" t="s">
         <v>456</v>
       </c>
-      <c r="C243" s="12"/>
-      <c r="D243" s="10"/>
-    </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C243" s="7"/>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A244" s="2" t="s">
         <v>455</v>
       </c>
       <c r="B244" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="C244" s="12"/>
-      <c r="D244" s="10"/>
-    </row>
-    <row r="245" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C244" s="7"/>
+    </row>
+    <row r="245" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A245" s="3" t="s">
         <v>458</v>
       </c>
       <c r="B245" s="3" t="s">
         <v>459</v>
       </c>
-      <c r="C245" s="12"/>
-      <c r="D245" s="10"/>
-    </row>
-    <row r="246" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C245" s="7"/>
+    </row>
+    <row r="246" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A246" s="3" t="s">
         <v>460</v>
       </c>
       <c r="B246" s="3" t="s">
         <v>461</v>
       </c>
-      <c r="C246" s="12"/>
-      <c r="D246" s="10"/>
-    </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C246" s="7"/>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A247" s="2" t="s">
         <v>460</v>
       </c>
       <c r="B247" s="2" t="s">
         <v>462</v>
       </c>
-      <c r="C247" s="12"/>
-      <c r="D247" s="10"/>
-    </row>
-    <row r="248" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C247" s="7"/>
+    </row>
+    <row r="248" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A248" s="3" t="s">
         <v>463</v>
       </c>
       <c r="B248" s="3" t="s">
         <v>464</v>
       </c>
-      <c r="C248" s="12"/>
-      <c r="D248" s="10"/>
-    </row>
-    <row r="249" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C248" s="7"/>
+    </row>
+    <row r="249" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A249" s="3" t="s">
         <v>465</v>
       </c>
       <c r="B249" s="3" t="s">
         <v>466</v>
       </c>
-      <c r="C249" s="12"/>
-      <c r="D249" s="10"/>
-    </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C249" s="7"/>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A250" s="2" t="s">
         <v>465</v>
       </c>
       <c r="B250" s="2" t="s">
         <v>467</v>
       </c>
-      <c r="C250" s="12"/>
-      <c r="D250" s="10"/>
-    </row>
-    <row r="251" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C250" s="7"/>
+    </row>
+    <row r="251" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A251" s="3" t="s">
         <v>468</v>
       </c>
       <c r="B251" s="3" t="s">
         <v>469</v>
       </c>
-      <c r="C251" s="12"/>
-      <c r="D251" s="10"/>
-    </row>
-    <row r="252" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C251" s="7"/>
+    </row>
+    <row r="252" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A252" s="3" t="s">
         <v>470</v>
       </c>
       <c r="B252" s="3" t="s">
         <v>471</v>
       </c>
-      <c r="C252" s="12"/>
-      <c r="D252" s="10"/>
-    </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C252" s="7"/>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A253" s="2" t="s">
         <v>470</v>
       </c>
       <c r="B253" s="2" t="s">
         <v>472</v>
       </c>
-      <c r="C253" s="12"/>
-      <c r="D253" s="10"/>
-    </row>
-    <row r="254" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C253" s="7"/>
+    </row>
+    <row r="254" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A254" s="3" t="s">
         <v>473</v>
       </c>
       <c r="B254" s="3" t="s">
         <v>474</v>
       </c>
-      <c r="D254" s="10"/>
-    </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A255" s="2" t="s">
         <v>475</v>
       </c>
       <c r="B255" s="2" t="s">
         <v>476</v>
       </c>
-      <c r="D255" s="10"/>
-    </row>
-    <row r="256" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="256" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A256" s="3" t="s">
         <v>477</v>
       </c>
       <c r="B256" s="3" t="s">
         <v>478</v>
       </c>
-      <c r="C256" s="13" t="s">
-        <v>506</v>
-      </c>
-      <c r="D256" s="10"/>
-    </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C256" s="8" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A257" s="2" t="s">
         <v>479</v>
       </c>
       <c r="B257" s="2" t="s">
         <v>480</v>
       </c>
-      <c r="C257" s="13"/>
-      <c r="D257" s="10"/>
-    </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C257" s="8"/>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A258" s="2" t="s">
         <v>481</v>
       </c>
       <c r="B258" s="2" t="s">
         <v>482</v>
       </c>
-      <c r="C258" s="13"/>
-      <c r="D258" s="10"/>
-    </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C258" s="8"/>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A259" s="2" t="s">
         <v>483</v>
       </c>
       <c r="B259" s="2" t="s">
         <v>484</v>
       </c>
-      <c r="C259" s="13"/>
-      <c r="D259" s="10"/>
-    </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C259" s="8"/>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A260" s="2" t="s">
         <v>485</v>
       </c>
       <c r="B260" s="2" t="s">
         <v>486</v>
       </c>
-      <c r="C260" s="13"/>
-      <c r="D260" s="10"/>
-    </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C260" s="8"/>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A261" s="2" t="s">
         <v>487</v>
       </c>
       <c r="B261" s="2" t="s">
         <v>488</v>
       </c>
-      <c r="C261" s="13"/>
-      <c r="D261" s="10"/>
-    </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C261" s="8"/>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A262" s="2" t="s">
         <v>489</v>
       </c>
       <c r="B262" s="2" t="s">
         <v>490</v>
       </c>
-      <c r="C262" s="13"/>
-      <c r="D262" s="10"/>
-    </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C262" s="8"/>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A263" s="2" t="s">
         <v>491</v>
       </c>
       <c r="B263" s="2" t="s">
         <v>492</v>
       </c>
-      <c r="C263" s="13"/>
-      <c r="D263" s="10"/>
-    </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C263" s="8"/>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A264" s="2" t="s">
         <v>493</v>
       </c>
       <c r="B264" s="2" t="s">
         <v>494</v>
       </c>
-      <c r="C264" s="13"/>
-      <c r="D264" s="10"/>
-    </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C264" s="8"/>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A265" s="2" t="s">
         <v>495</v>
       </c>
       <c r="B265" s="2" t="s">
         <v>496</v>
       </c>
-      <c r="C265" s="13"/>
-      <c r="D265" s="10"/>
-    </row>
-    <row r="266" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C265" s="8"/>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A266" s="2" t="s">
         <v>497</v>
       </c>
       <c r="B266" s="2" t="s">
         <v>498</v>
       </c>
-      <c r="C266" s="13"/>
-      <c r="D266" s="11"/>
-    </row>
-    <row r="267" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+      <c r="C266" s="8"/>
+    </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="D2:D66"/>
-    <mergeCell ref="D67:D77"/>
+  <mergeCells count="4">
     <mergeCell ref="C207:C253"/>
     <mergeCell ref="C256:C266"/>
     <mergeCell ref="C176:C178"/>
-    <mergeCell ref="D78:D138"/>
-    <mergeCell ref="D139:D266"/>
     <mergeCell ref="C74:C77"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>